<commit_message>
automatização finalizada e com as devidas recomendações funcionará corretamente
</commit_message>
<xml_diff>
--- a/leitor_cnpj/cnpj_ler.xlsx
+++ b/leitor_cnpj/cnpj_ler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sooretama-my.sharepoint.com/personal/larissa_sooretama_net/Documents/Área de Trabalho/Laryssa/projetos/leitor_cnpj/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{709F0036-805F-4F33-AA77-C391BCE19A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DBF6D813-FC70-4398-87CF-EBD1D5435C4B}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="8_{709F0036-805F-4F33-AA77-C391BCE19A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{430D791F-D6BF-4F34-8725-AF5B4293EFC4}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{37C2171E-6CAA-4AD4-B972-8A4C236EFED4}"/>
   </bookViews>
@@ -424,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA671B13-CC2B-465F-A4B8-4FCCEBAFB4A3}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,13 +446,24 @@
       </c>
     </row>
     <row r="3" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1">
+        <v>1612155000141</v>
+      </c>
     </row>
     <row r="4" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1">
+        <v>28129260000938</v>
+      </c>
     </row>
     <row r="5" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1">
+        <v>52123916001457</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>89425888000541</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
atualizações do dia 04/06
</commit_message>
<xml_diff>
--- a/leitor_cnpj/cnpj_ler.xlsx
+++ b/leitor_cnpj/cnpj_ler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sooretama-my.sharepoint.com/personal/larissa_sooretama_net/Documents/Área de Trabalho/Laryssa/projetos/leitor_cnpj/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="8_{709F0036-805F-4F33-AA77-C391BCE19A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45E48EA7-4F4D-4188-BEA4-C5459109FC03}"/>
+  <xr:revisionPtr revIDLastSave="78" documentId="8_{709F0036-805F-4F33-AA77-C391BCE19A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C482DB8E-D862-46F7-AD0D-A457097FFDE7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{37C2171E-6CAA-4AD4-B972-8A4C236EFED4}"/>
   </bookViews>
@@ -10154,8 +10154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA671B13-CC2B-465F-A4B8-4FCCEBAFB4A3}">
   <dimension ref="A1:A3245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A241" workbookViewId="0">
-      <selection activeCell="A270" sqref="A270"/>
+    <sheetView tabSelected="1" topLeftCell="A1782" workbookViewId="0">
+      <selection activeCell="A1800" sqref="A2:XFD1800"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>